<commit_message>
Pushed condition and observation profiles
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cbs-birthsex.xlsx
+++ b/output/StructureDefinition-cbs-birthsex.xlsx
@@ -254,7 +254,7 @@
     <t>Code for sex assigned at birth</t>
   </si>
   <si>
-    <t>https://phinvads.cdc.gov/vads/ViewValueSet.action?oid=2.16.840.1.114222.4.11.1038</t>
+    <t>http://phinvads.cdc.gov/vads/ViewValueSet.action?oid=2.16.840.1.114222.4.11.1038</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="27.96484375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="79.58984375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="78.65625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Fixed component slicing on cbs-observation
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cbs-birthsex.xlsx
+++ b/output/StructureDefinition-cbs-birthsex.xlsx
@@ -254,7 +254,7 @@
     <t>Code for sex assigned at birth</t>
   </si>
   <si>
-    <t>http://phinvads.cdc.gov/vads/ViewValueSet.action?oid=2.16.840.1.114222.4.11.1038</t>
+    <t>http://phinvads.cdc.gov/fhir/ValueSet/2.16.840.1.114222.4.11.1038</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="27.96484375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="78.65625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="63.4453125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>

</xml_diff>